<commit_message>
added config mode selector
</commit_message>
<xml_diff>
--- a/public/hercules.xlsx
+++ b/public/hercules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Electron\remoteHercules\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DFFE2C2-9D7F-492F-AC1F-9818E45D51C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{237AD4F4-3435-421B-9F20-192C01055E27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2070" yWindow="1035" windowWidth="20055" windowHeight="17970" xr2:uid="{34B49229-1ECB-4DC7-BFE8-A0B06FFFBA25}"/>
+    <workbookView xWindow="13875" yWindow="2445" windowWidth="20055" windowHeight="17970" xr2:uid="{34B49229-1ECB-4DC7-BFE8-A0B06FFFBA25}"/>
   </bookViews>
   <sheets>
     <sheet name="midimap" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="77">
   <si>
     <t>cc</t>
   </si>
@@ -264,6 +264,9 @@
   </si>
   <si>
     <t>cwxLoopBtnR</t>
+  </si>
+  <si>
+    <t>configMode</t>
   </si>
 </sst>
 </file>
@@ -640,8 +643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D956A4D3-4253-45EA-9BF7-F7A3D3B9B38F}">
   <dimension ref="A1:R51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J51" sqref="J51"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2016,8 +2019,11 @@
         <f t="shared" si="0"/>
         <v>1|3</v>
       </c>
+      <c r="J31" t="s">
+        <v>76</v>
+      </c>
       <c r="K31" s="8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L31" s="8">
         <v>0</v>
@@ -2805,7 +2811,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F485914A-B60F-4164-B1CA-5A2A7FA4A8F9}">
           <x14:formula1>
-            <xm:f>functions!$A$2:$A$63</xm:f>
+            <xm:f>functions!$A$2:$A$64</xm:f>
           </x14:formula1>
           <xm:sqref>J51 J1:J49</xm:sqref>
         </x14:dataValidation>
@@ -2817,10 +2823,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3731D5E7-1A5C-4C46-A916-A5AC3FB36FB7}">
-  <dimension ref="A1:A18"/>
+  <dimension ref="A1:A19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2841,81 +2847,86 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>57</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added slice toggle and tried create sliced...
</commit_message>
<xml_diff>
--- a/public/hercules.xlsx
+++ b/public/hercules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Electron\remoteHercules\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F085E56-5D81-4888-86BA-1691E4E9A276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDADBD7A-50AC-42CE-8C90-7F5D16016053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16320" yWindow="510" windowWidth="25545" windowHeight="14775" activeTab="1" xr2:uid="{34B49229-1ECB-4DC7-BFE8-A0B06FFFBA25}"/>
+    <workbookView xWindow="22080" yWindow="2550" windowWidth="25545" windowHeight="14775" activeTab="2" xr2:uid="{34B49229-1ECB-4DC7-BFE8-A0B06FFFBA25}"/>
   </bookViews>
   <sheets>
     <sheet name="midimap" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="90">
   <si>
     <t>cc</t>
   </si>
@@ -272,9 +272,6 @@
     <t>Change the RIT of Slice 0 or 1 with left or right Tempo Fader</t>
   </si>
   <si>
-    <t>Remove both Slices and create new Slice A and Slice B</t>
-  </si>
-  <si>
     <t>Jump through the different predefined step width to make the frequency change</t>
   </si>
   <si>
@@ -300,6 +297,15 @@
   </si>
   <si>
     <t>Enable/Disable config mode to select up to 8 different config&lt;nr&gt;-jsons using Hot CUE/Loop and Btns1-4</t>
+  </si>
+  <si>
+    <t>toggleSlices</t>
+  </si>
+  <si>
+    <t>Toggle order of the two slices</t>
+  </si>
+  <si>
+    <t>Remove both Slices and create new (buggy)</t>
   </si>
 </sst>
 </file>
@@ -677,7 +683,7 @@
   <dimension ref="A1:R51"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1078,7 +1084,7 @@
         <v>0|3</v>
       </c>
       <c r="J9" t="s">
-        <v>62</v>
+        <v>87</v>
       </c>
       <c r="K9" s="8">
         <v>2</v>
@@ -2853,7 +2859,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F485914A-B60F-4164-B1CA-5A2A7FA4A8F9}">
           <x14:formula1>
-            <xm:f>functions!$A$2:$A$66</xm:f>
+            <xm:f>functions!$A$2:$A$67</xm:f>
           </x14:formula1>
           <xm:sqref>J51 J1:J49</xm:sqref>
         </x14:dataValidation>
@@ -2867,8 +2873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F356390-C5A1-4956-8118-11B48E316739}">
   <dimension ref="A1:R51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5038,7 +5044,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9A2D9150-9195-4181-AAD2-A5D7BB7BA7B9}">
           <x14:formula1>
-            <xm:f>functions!$A$2:$A$66</xm:f>
+            <xm:f>functions!$A$2:$A$67</xm:f>
           </x14:formula1>
           <xm:sqref>J51 J1:J49</xm:sqref>
         </x14:dataValidation>
@@ -5050,10 +5056,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3731D5E7-1A5C-4C46-A916-A5AC3FB36FB7}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5080,7 +5086,7 @@
         <v>67</v>
       </c>
       <c r="D3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -5088,7 +5094,7 @@
         <v>65</v>
       </c>
       <c r="D4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -5168,7 +5174,7 @@
         <v>62</v>
       </c>
       <c r="D14" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -5176,7 +5182,7 @@
         <v>54</v>
       </c>
       <c r="D15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -5184,7 +5190,7 @@
         <v>66</v>
       </c>
       <c r="D16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -5192,7 +5198,7 @@
         <v>56</v>
       </c>
       <c r="D17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -5200,31 +5206,39 @@
         <v>57</v>
       </c>
       <c r="D18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>53</v>
+        <v>87</v>
       </c>
       <c r="D19" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D20" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>48</v>
       </c>
-      <c r="D21" t="s">
-        <v>85</v>
+      <c r="D22" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>